<commit_message>
work chapter 1 to 6 - unclean
</commit_message>
<xml_diff>
--- a/osi-blockchain/OSI_Blockchain.xlsx
+++ b/osi-blockchain/OSI_Blockchain.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mwea-my.sharepoint.com/personal/sebastian_kanz_maibornwolff_de/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastianka\Git\thesis\osi-blockchain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{72ADD5C3-6DA7-4BF2-803A-5A5EC6727C5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1D878F3-3146-4CC6-B90E-442D13923925}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA8C7F-F5E0-468E-9A3A-6757DBEAF6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{299674EF-571D-4AD6-B432-0A4210275200}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Application</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Consensus</t>
   </si>
   <si>
-    <t>dApps</t>
-  </si>
-  <si>
     <t>Transportorientiert</t>
   </si>
   <si>
@@ -87,13 +84,19 @@
     <t>Virtual Machine</t>
   </si>
   <si>
-    <t>Smart Contracts</t>
-  </si>
-  <si>
     <t>Browser, Wallet, Block-Explorer</t>
   </si>
   <si>
     <t>(User Interface)</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>TCP / UDP</t>
+  </si>
+  <si>
+    <t>dApps (Smart Contracts) / Top-Level APIs</t>
   </si>
 </sst>
 </file>
@@ -132,10 +135,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,160 +460,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26187E82-9971-4380-8379-DE527EE25783}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D7" sqref="D3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="3"/>
-    <col min="3" max="3" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="3"/>
+    <col min="1" max="2" width="11.5546875" style="2"/>
+    <col min="3" max="3" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>6</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>3</v>
+      <c r="A8" s="2">
+        <v>2</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>2</v>
+      <c r="A9" s="2">
+        <v>1</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="5">
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="E7:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100083C29D1F8A4C34185509A8A1AE40315" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="efa01d203642e3ad2227c718847520cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="52395fc8-4895-476e-8332-158722e0cc2e" xmlns:ns4="ab5c3af9-14fb-4434-bd5c-9bbeb2620a41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0cea346c58a2c34bb22d0e0b9a545457" ns3:_="" ns4:_="">
     <xsd:import namespace="52395fc8-4895-476e-8332-158722e0cc2e"/>
@@ -813,22 +825,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FCFB047-AAAE-45D5-8C57-F9462EE12188}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C60C9C-4C72-4110-A07E-CF78627FE496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3531E071-2424-46F5-A963-1930736AF9E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -845,21 +859,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2C60C9C-4C72-4110-A07E-CF78627FE496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FCFB047-AAAE-45D5-8C57-F9462EE12188}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>